<commit_message>
p1 p2 complete; button pos change;
</commit_message>
<xml_diff>
--- a/数据.xlsx
+++ b/数据.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153">
   <si>
     <t>采集数据</t>
   </si>
@@ -104,6 +104,9 @@
     <t>球员信息</t>
   </si>
   <si>
+    <t>主队球员</t>
+  </si>
+  <si>
     <t>player0</t>
   </si>
   <si>
@@ -125,7 +128,7 @@
     <t>位置（守门员、后卫、中场、前锋）</t>
   </si>
   <si>
-    <t>id</t>
+    <t>tid</t>
   </si>
   <si>
     <t>pid</t>
@@ -143,6 +146,9 @@
     <t>其他球员</t>
   </si>
   <si>
+    <t>客队球员</t>
+  </si>
+  <si>
     <t>sequences</t>
   </si>
   <si>
@@ -276,9 +282,6 @@
   </si>
   <si>
     <t>具体内容</t>
-  </si>
-  <si>
-    <t>tid</t>
   </si>
   <si>
     <t>队伍编号（需要官方提供队伍列表，我们建立数据库，为队伍编号）</t>
@@ -478,10 +481,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -558,16 +561,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -581,15 +597,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,25 +620,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,10 +643,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -665,7 +691,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -674,29 +700,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -711,13 +714,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,25 +756,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,7 +774,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,7 +882,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,109 +894,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,15 +1109,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1148,6 +1142,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1162,15 +1174,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1179,10 +1182,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1191,137 +1194,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1415,9 +1418,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1433,45 +1433,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1490,46 +1496,49 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1851,10 +1860,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:J65"/>
+  <dimension ref="B2:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1895,10 +1904,10 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="25"/>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="54" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1912,8 +1921,8 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54" t="s">
+      <c r="I4" s="55"/>
+      <c r="J4" s="55" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1927,10 +1936,10 @@
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
       <c r="H5" s="30"/>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="56" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1944,10 +1953,10 @@
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="56" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1961,10 +1970,10 @@
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="55" t="s">
+      <c r="J7" s="56" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1978,10 +1987,10 @@
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="30"/>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="56" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1995,15 +2004,15 @@
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="56" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="31"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="30" t="s">
         <v>19</v>
       </c>
@@ -2012,15 +2021,15 @@
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="56" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="31"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="29" t="s">
         <v>21</v>
       </c>
@@ -2033,15 +2042,15 @@
       <c r="J11" s="56"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="57" t="s">
         <v>23</v>
       </c>
@@ -2050,15 +2059,15 @@
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="35"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="57" t="s">
         <v>23</v>
       </c>
@@ -2075,564 +2084,578 @@
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="54"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="59" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="28"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="29" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="60" t="s">
+      <c r="H15" s="29"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="61" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="28"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="57" t="s">
-        <v>23</v>
-      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="58" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="28"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="33" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="57" t="s">
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="28"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="33" t="s">
+      <c r="J18" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="57" t="s">
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="28"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="33" t="s">
+      <c r="J19" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="57" t="s">
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="58" t="s">
+      <c r="J20" s="62" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="28"/>
-      <c r="C20" s="29" t="s">
+    <row r="21" spans="2:10">
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="60" t="s">
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="35"/>
-      <c r="C21" s="39" t="s">
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="62" t="s">
+    </row>
+    <row r="23" customFormat="1" spans="2:10">
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="26" t="s">
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="59" t="s">
+    </row>
+    <row r="24" customFormat="1" spans="2:10">
+      <c r="B24" s="36"/>
+      <c r="C24" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="28"/>
-      <c r="C23" s="29" t="s">
+    <row r="25" spans="2:10">
+      <c r="B25" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="60" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="59" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="28"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="58" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="28"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="64" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="28"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="66" t="s">
-        <v>51</v>
+      <c r="C26" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="61" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="28"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="66" t="s">
-        <v>52</v>
+      <c r="C27" s="41"/>
+      <c r="D27" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="58" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="28"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" s="66" t="s">
-        <v>53</v>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="62" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="28"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="43"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="65"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="42"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="65" t="s">
+        <v>13</v>
+      </c>
       <c r="J29" s="66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="28"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="46"/>
-      <c r="I30" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30" s="46" t="s">
-        <v>58</v>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="66" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="28"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="H31" s="46"/>
-      <c r="I31" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" s="46" t="s">
-        <v>60</v>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="42"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="66" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="28"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="44"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="42"/>
+      <c r="H32" s="43"/>
       <c r="I32" s="65"/>
       <c r="J32" s="66" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="28"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="48"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="46" t="s">
-        <v>64</v>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="45"/>
+      <c r="I33" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" s="45" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="28"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="I34" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="69" t="s">
-        <v>66</v>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="45"/>
+      <c r="I34" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="45" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="28"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I35" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="69" t="s">
-        <v>68</v>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="42"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="66" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="28"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="48"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" s="47"/>
       <c r="I36" s="67"/>
-      <c r="J36" s="46" t="s">
-        <v>70</v>
+      <c r="J36" s="45" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="28"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="H37" s="48"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="46" t="s">
-        <v>72</v>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I37" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="69" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="28"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="41" t="s">
-        <v>73</v>
-      </c>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="41"/>
       <c r="G38" s="41"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="64" t="s">
-        <v>74</v>
+      <c r="H38" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" s="69" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="28"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="41" t="s">
-        <v>40</v>
-      </c>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="63"/>
-      <c r="J39" s="64" t="s">
-        <v>75</v>
+      <c r="G39" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" s="47"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="45" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="28"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="58" t="s">
-        <v>76</v>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="H40" s="47"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="45" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="28"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="64" t="s">
-        <v>78</v>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="62" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="28"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="J42" s="64" t="s">
-        <v>80</v>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="28"/>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="41"/>
+      <c r="D43" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="28"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" s="62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="28"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="60" t="s">
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="62" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
-      <c r="B44" s="35"/>
-      <c r="C44" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="62" t="s">
+    <row r="46" spans="2:10">
+      <c r="B46" s="28"/>
+      <c r="C46" s="29" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="45" spans="2:10">
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-    </row>
-    <row r="46" spans="2:10">
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="61" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="47" spans="2:10">
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
       <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="71" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
     </row>
     <row r="50" spans="2:10">
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
     </row>
     <row r="51" spans="2:10">
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
     </row>
     <row r="52" spans="2:10">
       <c r="B52" s="51"/>
@@ -2668,128 +2691,161 @@
       <c r="J54" s="51"/>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" s="51"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="51"/>
-      <c r="H55" s="51"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="51"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="51"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="51"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="51"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="51"/>
-      <c r="G57" s="51"/>
-      <c r="H57" s="51"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="51"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="51"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="51"/>
-      <c r="G58" s="51"/>
-      <c r="H58" s="51"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="51"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="51"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="51"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="51"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" s="51"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="51"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="51"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="51"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="52"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
     </row>
     <row r="62" spans="2:10">
-      <c r="B62" s="51"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="51"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
     </row>
     <row r="63" spans="2:10">
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="51"/>
-      <c r="F63" s="51"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="51"/>
-      <c r="I63" s="51"/>
-      <c r="J63" s="51"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
     </row>
     <row r="64" spans="2:10">
-      <c r="B64" s="51"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
-      <c r="E64" s="51"/>
-      <c r="F64" s="51"/>
-      <c r="G64" s="51"/>
-      <c r="H64" s="51"/>
-      <c r="I64" s="51"/>
-      <c r="J64" s="51"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="52"/>
+      <c r="F64" s="52"/>
+      <c r="G64" s="52"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
     </row>
     <row r="65" spans="2:10">
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="50"/>
+      <c r="B65" s="52"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="52"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="52"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="52"/>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="52"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="52"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
+      <c r="H67" s="52"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="57">
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
@@ -2805,44 +2861,48 @@
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="E28:H28"/>
     <mergeCell ref="F29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="F35:H35"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="C47:H47"/>
     <mergeCell ref="B5:B13"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="B23:B44"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="B26:B47"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C24:C42"/>
-    <mergeCell ref="D25:D39"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E26:E37"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F33:F37"/>
-    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="C16:C23"/>
+    <mergeCell ref="C27:C45"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="D28:D42"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E29:E40"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G37:G38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -2869,17 +2929,17 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>3</v>
@@ -2887,452 +2947,452 @@
     </row>
     <row r="4" ht="40.5" spans="2:4">
       <c r="B4" s="7" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" ht="40.5" spans="2:4">
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="27" spans="2:4">
       <c r="B6" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="14.25" spans="2:4">
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="14"/>
     </row>
     <row r="8" ht="14.25" spans="2:4">
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="14"/>
     </row>
     <row r="9" ht="14.25" spans="2:4">
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9" s="14"/>
     </row>
     <row r="10" ht="14.25" spans="2:4">
       <c r="B10" s="12"/>
       <c r="C10" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D10" s="14"/>
     </row>
     <row r="11" ht="14.25" spans="2:4">
       <c r="B11" s="12"/>
       <c r="C11" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D11" s="14"/>
     </row>
     <row r="12" ht="14.25" spans="2:4">
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" s="14"/>
     </row>
     <row r="13" ht="14.25" spans="2:4">
       <c r="B13" s="12"/>
       <c r="C13" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D13" s="14"/>
     </row>
     <row r="14" ht="14.25" spans="2:4">
       <c r="B14" s="12"/>
       <c r="C14" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D14" s="14"/>
     </row>
     <row r="15" ht="14.25" spans="2:4">
       <c r="B15" s="12"/>
       <c r="C15" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D15" s="14"/>
     </row>
     <row r="16" ht="14.25" spans="2:4">
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D16" s="14"/>
     </row>
     <row r="17" ht="14.25" spans="2:4">
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D17" s="14"/>
     </row>
     <row r="18" ht="14.25" spans="2:4">
       <c r="B18" s="12"/>
       <c r="C18" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D18" s="14"/>
     </row>
     <row r="19" ht="14.25" spans="2:4">
       <c r="B19" s="12"/>
       <c r="C19" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19" s="14"/>
     </row>
     <row r="20" ht="14.25" spans="2:4">
       <c r="B20" s="12"/>
       <c r="C20" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D20" s="14"/>
     </row>
     <row r="21" ht="14.25" spans="2:4">
       <c r="B21" s="12"/>
       <c r="C21" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D21" s="14"/>
     </row>
     <row r="22" ht="14.25" spans="2:4">
       <c r="B22" s="12"/>
       <c r="C22" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D22" s="14"/>
     </row>
     <row r="23" ht="14.25" spans="2:4">
       <c r="B23" s="12"/>
       <c r="C23" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="15"/>
     </row>
     <row r="24" ht="14.25" spans="2:4">
       <c r="B24" s="12"/>
       <c r="C24" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D24" s="15"/>
     </row>
     <row r="25" ht="14.25" spans="2:4">
       <c r="B25" s="12"/>
       <c r="C25" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D25" s="15"/>
     </row>
     <row r="26" ht="14.25" spans="2:4">
       <c r="B26" s="12"/>
       <c r="C26" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D26" s="15"/>
     </row>
     <row r="27" ht="14.25" spans="2:4">
       <c r="B27" s="12"/>
       <c r="C27" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D27" s="15"/>
     </row>
     <row r="28" ht="14.25" spans="2:4">
       <c r="B28" s="12"/>
       <c r="C28" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D28" s="15"/>
     </row>
     <row r="29" ht="14.25" spans="2:4">
       <c r="B29" s="12"/>
       <c r="C29" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D29" s="15"/>
     </row>
     <row r="30" ht="14.25" spans="2:4">
       <c r="B30" s="12"/>
       <c r="C30" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D30" s="15"/>
     </row>
     <row r="31" ht="14.25" spans="2:4">
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D31" s="15"/>
     </row>
     <row r="32" ht="14.25" spans="2:4">
       <c r="B32" s="12"/>
       <c r="C32" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D32" s="15"/>
     </row>
     <row r="33" ht="14.25" spans="2:4">
       <c r="B33" s="12"/>
       <c r="C33" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D33" s="15"/>
     </row>
     <row r="34" ht="14.25" spans="2:4">
       <c r="B34" s="12"/>
       <c r="C34" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D34" s="15"/>
     </row>
     <row r="35" ht="14.25" spans="2:4">
       <c r="B35" s="12"/>
       <c r="C35" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D35" s="15"/>
     </row>
     <row r="36" ht="14.25" spans="2:4">
       <c r="B36" s="12"/>
       <c r="C36" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D36" s="15"/>
     </row>
     <row r="37" ht="14.25" spans="2:4">
       <c r="B37" s="12"/>
       <c r="C37" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D37" s="15"/>
     </row>
     <row r="38" ht="14.25" spans="2:4">
       <c r="B38" s="12"/>
       <c r="C38" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D38" s="15"/>
     </row>
     <row r="39" ht="14.25" spans="2:4">
       <c r="B39" s="12"/>
       <c r="C39" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D39" s="15"/>
     </row>
     <row r="40" ht="14.25" spans="2:4">
       <c r="B40" s="12"/>
       <c r="C40" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" s="15"/>
     </row>
     <row r="41" ht="14.25" spans="2:4">
       <c r="B41" s="12"/>
       <c r="C41" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D41" s="15"/>
     </row>
     <row r="42" ht="14.25" spans="2:4">
       <c r="B42" s="12"/>
       <c r="C42" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D42" s="15"/>
     </row>
     <row r="43" ht="14.25" spans="2:4">
       <c r="B43" s="16"/>
       <c r="C43" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D43" s="18"/>
     </row>
     <row r="44" ht="14.25" spans="2:4">
       <c r="B44" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D44" s="20"/>
     </row>
     <row r="45" ht="14.25" spans="2:4">
       <c r="B45" s="12"/>
       <c r="C45" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="15"/>
     </row>
     <row r="46" ht="14.25" spans="2:4">
       <c r="B46" s="12"/>
       <c r="C46" s="21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D46" s="15"/>
     </row>
     <row r="47" ht="14.25" spans="2:4">
       <c r="B47" s="12"/>
       <c r="C47" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D47" s="15"/>
     </row>
     <row r="48" ht="14.25" spans="2:4">
       <c r="B48" s="12"/>
       <c r="C48" s="21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D48" s="15"/>
     </row>
     <row r="49" ht="14.25" spans="2:4">
       <c r="B49" s="12"/>
       <c r="C49" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D49" s="15"/>
     </row>
     <row r="50" ht="14.25" spans="2:4">
       <c r="B50" s="12"/>
       <c r="C50" s="21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D50" s="15"/>
     </row>
     <row r="51" ht="14.25" spans="2:4">
       <c r="B51" s="12"/>
       <c r="C51" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D51" s="15"/>
     </row>
     <row r="52" ht="14.25" spans="2:4">
       <c r="B52" s="12"/>
       <c r="C52" s="21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D52" s="15"/>
     </row>
     <row r="53" ht="14.25" spans="2:4">
       <c r="B53" s="12"/>
       <c r="C53" s="21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D53" s="15"/>
     </row>
     <row r="54" ht="14.25" spans="2:4">
       <c r="B54" s="12"/>
       <c r="C54" s="21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D54" s="15"/>
     </row>
     <row r="55" ht="14.25" spans="2:4">
       <c r="B55" s="12"/>
       <c r="C55" s="21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D55" s="15"/>
     </row>
     <row r="56" ht="14.25" spans="2:4">
       <c r="B56" s="12"/>
       <c r="C56" s="21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D56" s="15"/>
     </row>
     <row r="57" ht="14.25" spans="2:4">
       <c r="B57" s="12"/>
       <c r="C57" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D57" s="15"/>
     </row>
     <row r="58" ht="14.25" spans="2:4">
       <c r="B58" s="12"/>
       <c r="C58" s="21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D58" s="15"/>
     </row>
     <row r="59" ht="14.25" spans="2:4">
       <c r="B59" s="12"/>
       <c r="C59" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D59" s="15"/>
     </row>
     <row r="60" ht="14.25" spans="2:4">
       <c r="B60" s="12"/>
       <c r="C60" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D60" s="15"/>
     </row>
     <row r="61" ht="14.25" spans="2:4">
       <c r="B61" s="12"/>
       <c r="C61" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D61" s="15"/>
     </row>
     <row r="62" ht="14.25" spans="2:4">
       <c r="B62" s="12"/>
       <c r="C62" s="21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D62" s="15"/>
     </row>
     <row r="63" ht="14.25" spans="2:4">
       <c r="B63" s="12"/>
       <c r="C63" s="21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D63" s="15"/>
     </row>
     <row r="64" ht="14.25" spans="2:4">
       <c r="B64" s="12"/>
       <c r="C64" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D64" s="15"/>
     </row>
     <row r="65" ht="14.25" spans="2:4">
       <c r="B65" s="12"/>
       <c r="C65" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D65" s="15"/>
     </row>
     <row r="66" ht="14.25" spans="2:4">
       <c r="B66" s="16"/>
       <c r="C66" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D66" s="18"/>
     </row>

</xml_diff>